<commit_message>
Accounted for diagonals when choosing new path
</commit_message>
<xml_diff>
--- a/Resources/Grid Navigation Paths.xlsx
+++ b/Resources/Grid Navigation Paths.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="32">
   <si>
     <t>→</t>
   </si>
@@ -97,12 +97,6 @@
     <t>Checking each seen twice</t>
   </si>
   <si>
-    <t>Check each seen only once, Method 1.1</t>
-  </si>
-  <si>
-    <t>Check each seen only once, Method 2.1</t>
-  </si>
-  <si>
     <t>Visit each point</t>
   </si>
   <si>
@@ -121,19 +115,13 @@
     <t>Been Min Turns: 14</t>
   </si>
   <si>
-    <t>Check each seen only once, Method 1.0 (Incomplete)</t>
-  </si>
-  <si>
-    <t>Check each seen only once, Method 2.0 (Incomplete)</t>
-  </si>
-  <si>
     <t>Seen</t>
   </si>
   <si>
     <t>Visited</t>
   </si>
   <si>
-    <t>Check each seen only once, Method 2.2</t>
+    <t>Check each seen only once</t>
   </si>
 </sst>
 </file>
@@ -253,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -287,7 +275,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +795,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="J1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -849,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -928,7 +915,7 @@
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
       <c r="S4" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1003,7 +990,7 @@
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="S6" s="23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1147,9 +1134,6 @@
       <c r="J11" t="s">
         <v>31</v>
       </c>
-      <c r="S11" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1255,19 +1239,19 @@
       <c r="J14" s="7"/>
       <c r="K14" s="6"/>
       <c r="L14" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="6"/>
       <c r="O14" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="6"/>
       <c r="U14" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V14" s="11"/>
       <c r="W14" s="6"/>
@@ -1538,14 +1522,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J22" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="22" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
@@ -1642,7 +1619,7 @@
       <c r="S26" s="7"/>
       <c r="T26" s="6"/>
       <c r="U26" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="V26" s="10" t="s">
         <v>8</v>
@@ -1792,9 +1769,6 @@
     </row>
     <row r="32" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" t="s">
-        <v>35</v>
-      </c>
       <c r="S33" s="20"/>
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
@@ -1813,14 +1787,14 @@
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
-      <c r="W34" s="20"/>
-      <c r="X34" s="20"/>
-      <c r="Y34" s="20"/>
-      <c r="Z34" s="20"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
     </row>
     <row r="35" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J35" s="10" t="s">
@@ -1835,21 +1809,27 @@
       <c r="Q35" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="S35" s="17"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="25"/>
-      <c r="V35" s="25"/>
-      <c r="W35" s="25"/>
-      <c r="X35" s="25"/>
-      <c r="Y35" s="25"/>
-      <c r="Z35" s="17"/>
+      <c r="S35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J36" s="7"/>
       <c r="K36" s="6">
         <v>1</v>
       </c>
-      <c r="L36" s="11"/>
+      <c r="L36" s="11">
+        <v>1</v>
+      </c>
       <c r="M36" s="11">
         <v>1</v>
       </c>
@@ -1861,14 +1841,22 @@
         <v>1</v>
       </c>
       <c r="Q36" s="7"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="17"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="6">
+        <v>1</v>
+      </c>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11">
+        <v>1</v>
+      </c>
+      <c r="W36" s="6">
+        <v>1</v>
+      </c>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="7"/>
     </row>
     <row r="37" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J37" s="7"/>
@@ -1885,14 +1873,14 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="7"/>
-      <c r="S37" s="25"/>
-      <c r="T37" s="25"/>
-      <c r="U37" s="17"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="17"/>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="7"/>
     </row>
     <row r="38" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J38" s="7"/>
@@ -1907,14 +1895,20 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="7"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="25"/>
-      <c r="U38" s="25"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="25"/>
-      <c r="X38" s="25"/>
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="6">
+        <v>1</v>
+      </c>
+      <c r="U38" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="V38" s="24"/>
+      <c r="W38" s="12"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="7"/>
     </row>
     <row r="39" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J39" s="7"/>
@@ -1929,14 +1923,18 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="7"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="25"/>
-      <c r="U39" s="25"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="25"/>
-      <c r="X39" s="25"/>
-      <c r="Y39" s="25"/>
-      <c r="Z39" s="25"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="6">
+        <v>1</v>
+      </c>
+      <c r="U39" s="7"/>
+      <c r="V39" s="11">
+        <v>1</v>
+      </c>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="7"/>
     </row>
     <row r="40" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J40" s="7"/>
@@ -1951,14 +1949,16 @@
       <c r="O40" s="8"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="7"/>
-      <c r="S40" s="25"/>
-      <c r="T40" s="25"/>
-      <c r="U40" s="25"/>
-      <c r="V40" s="20"/>
-      <c r="W40" s="25"/>
-      <c r="X40" s="17"/>
-      <c r="Y40" s="25"/>
-      <c r="Z40" s="25"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="6">
+        <v>1</v>
+      </c>
+      <c r="U40" s="7"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="6"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="7"/>
     </row>
     <row r="41" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J41" s="7"/>
@@ -1975,14 +1975,20 @@
       <c r="Q41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="17"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="17"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="6">
+        <v>1</v>
+      </c>
+      <c r="U41" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J42" s="10" t="s">
@@ -1995,14 +2001,16 @@
       <c r="O42" s="11"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
-      <c r="S42" s="17"/>
-      <c r="T42" s="25"/>
-      <c r="U42" s="20"/>
-      <c r="V42" s="20"/>
-      <c r="W42" s="20"/>
-      <c r="X42" s="20"/>
-      <c r="Y42" s="20"/>
-      <c r="Z42" s="20"/>
+      <c r="S42" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T42" s="6"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2442,10 +2450,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>